<commit_message>
Pushing Ebay Shortened Ver
</commit_message>
<xml_diff>
--- a/Manipulated data.xlsx
+++ b/Manipulated data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,1093 +441,738 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>PKR in price</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>datetime</t>
+          <t>$ in price</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Apple iPhone 8 (Great Condition) Factory Unlocked, AT&amp;T, T-Mobile or Verizon</t>
+          <t>Samsung Galaxy S7 G930F 32GB Black White Gold Silver Unlocked - GOOD ⭐</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>46471.1526958</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>80.44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Apple iPad A1432 Mini 16GB Wi-Fi 7.9 inch Blue Space Gray Silver - Excellent</t>
+          <t>Samsung Galaxy S21 | S21+ Plus 5G - 128GB - Unlocked | Verizon | T-Mobile | AT&amp;T</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16755.9783858</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>204.95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Apple - iPhone 15 - 128GB - Unlocked - Factory Warranty - All Colors</t>
+          <t>Samsung S20+ Plus 5G Unlocked G986U 128GB Android Smartphone Spot</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>258845.92598</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>New ListingApple iPhone 14 Pro - 512GB - Purple (Unlocked) (Read Description) DF1121</t>
+          <t>Samsung Galaxy S10e SM-G970U Verizon Unlocked 128GB Prism Black C</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>58444.53715</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>99.98999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 64GB 128GB Verizon T-Mobile AT&amp;T Unlocked Good Condition</t>
+          <t>Samsung G965 Galaxy S9+ Plus 64GB Unlocked Smartphone - Good</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>58867.02778</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>112.95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 - 128GB - A2111 Fully Unlocked - Pristine Condition - Smartphone</t>
+          <t>Samsung Galaxy S21 5G SM-G991 128GB Unlocked AT&amp;T Verizon T-Mobile S21 Very Good</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>63091.93408</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>224.98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 Pro Max  128gb Unlocked - Excellent</t>
+          <t>SAMSUNG Galaxy S23 Ultra SM-S918B/DS 5G 256GB/12GB Unlocked Sealed Brand New</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>201384.3836958</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>949</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2017 APPLE MACBOOK PRO 15 INCH TOUCHBAR 2.9GHz i7 16GB 500GB Pro 560 SAVE</t>
+          <t>Samsung Galaxy S10E G970U (UNLOCKED) ALL COLORS (Good)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>102806.0533</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>99%New Apple iPhone 4s - 16GB - White (Unlocked) A1387 (CDMA   GSM)</t>
+          <t>Samsung Galaxy S21 Ultra SM-G998U1 - 5G - 128GB Black Fully Unlocked GSM+CDMA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>13238.03974</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>319.99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Apple iPhone XR - 64GB 128GB 256GB - All Colors - Good Condition</t>
+          <t>Samsung Galaxy S9 | S9+ Plus 64GB 128GB 256GB - Unlocked Verizon T-Mobile AT&amp;T</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>55205.44231999999</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>99.95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Apple iPhone 6 16GB 64GB 128GB Factory Unlocked AT&amp;T Verizon TMobile Sprint Mint</t>
+          <t>Samsung G975 Galaxy S10 Plus 128GB Factory Unlocked Smartphone SHADOW SCREEN</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10703.09596</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>147.95</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 Unlocked 64GB 128GB 256GB | Verizon T-Mobile AT&amp;T | Very Good</t>
+          <t>Samsung Galaxy S20 | S20+ | S20 FE | S20 Ultra 5G 128GB - Unlocked Verizon AT&amp;T</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>107025.3263916</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>169.95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 mini 64GB Factory Unlocked AT&amp;T T-Mobile Verizon Fair Condition</t>
+          <t>Samsung Galaxy S20+ Plus 5G Unlocked G986U 128GB Android Smartphone Good</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>68992.719879</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>183.99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Apple iPhone 8 (Excellent Condition) Factory Unlocked, ATT, TMobile, Verizon GSM</t>
+          <t>Samsung Galaxy A40 64GB Unlocked Very Good Working Order But (Screen Crack)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>50696.0589958</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>36.56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 - 64GB | 128GB - (Unlocked) A2111 (CDMA + GSM) Smartphone - Good</t>
+          <t>Samsung Galaxy S20+ Plus 5G G986U Unlocked 128GB</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>73217.626179</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>179.99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Apple Macbook Pro 13" Laptop | UPGRADED i5 16GB RAM | 1TB HD | MacOS | WARRANTY</t>
+          <t>Samsung Galaxy S20 5G Unlocked G981U 128GB Android Smartphone Spot</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>50417.21518</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>99.23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 - 128GB - Black. Unlocked A2111 (CDMA + GSM) Good Condition</t>
+          <t>Samsung Galaxy A14 5G - 128GB (GSM UNLOCKED) 4GB RAM Dual Sim 6.6" Display NEW</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>58867.02778</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>198.99</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Apple iPhone 14 - 128GB/256GB/512GB - All Colors - Choose your Network</t>
+          <t>Samsung Galaxy A23 5G SM-A236U, 64GB, Black Unlocked T-Mobile AT&amp;T</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>129560.9765958</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>124.99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Apple Macbook Pro 13" Laptop i5 + 8GB RAM + 256GB SSD HD.  macOS High Sierra</t>
+          <t xml:space="preserve">Samsung Galaxy S10 S10e S10+ Plus 128GB 512GB Unlocked Verizon T-Mobile AT&amp;T </t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>50417.21518</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>124.85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Apple iPhone 14 Pro Max 128GB ( Unlocked)  US E Sim - Excellent</t>
+          <t>Samsung N960 Galaxy Note 9 128GB Unlocked Smartphone SHADOW SCREEN</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>247858.3529958</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>129.95</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 64/128/256GB -  Fully Unlocked - All colors - Used Condition</t>
+          <t xml:space="preserve">New ListingSamsung Galaxy Z Fold3 256GB Black </t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>84495.3093958</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>51</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 Pro Max 128/256/512GB AT&amp;T Sprint T-Mobile Unlocked Verizon Fair</t>
+          <t>Ghost/ Shadow LCD - Samsung Galaxy Note 20 Ultra 5G 128G N986U Unlocked</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>140827.3933958</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>127.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Apple iPhone X - 256 GB - All Colors - Fully Unlocked - Very Good Condition</t>
+          <t>Samsung Galaxy S22 5G 128GB 256GB - Unlocked Verizon T-Mobile AT&amp;T Cricket Metro</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46192.30888</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>329.95</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 64GB 128GB 256GB Fully Unlocked 5G Smartphone - Good</t>
+          <t>Samsung Galaxy A11 SM-A115U - 32GB - Black (Unlocked) (Single SIM)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>92945.1219958</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 64GB 128GB 256GB GSM UNLOCKED, VERIZON UNLOCKED Fair</t>
+          <t>Samsung Galaxy S10- 128GB - Unlocked SIM - SM-G973U - Fully Working! Fair!</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>67595.6841958</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>117.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Apple iPhone X | XR | XS | XS Max - 64GB 128GB 256GB - Verizon GSM Unlocked AT&amp;T</t>
+          <t>Samsung Galaxy S20+ Plus 5G Unlocked G986U 128GB Android Smartphone Good Shadow</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>54909.698879</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>174</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 mini 128GB Factory Unlocked AT&amp;T T-Mobile Verizon Fair Condition</t>
+          <t>Samsung Galaxy Note20 5G SM-N981U - 128GB -  (Unlocked) Shaded</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>108425.178679</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>199.99</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>New &amp; Sealed Apple Watch SE 40mm GPS + Cellular Gold with Starlight Sports Band</t>
+          <t>Samsung Galaxy S20 Ultra 5G Unlocked G988U 128GB Android Good Shadow</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>47868.18837899999</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>205</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Apple iPhone 6 Plus 16GB 64GB Factory Unlocked AT&amp;T T-mobile Verizon Good</t>
+          <t>Samsung Galaxy S8 | S8 Plus G950U | G955U - 64GB - (Unlocked) Good</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>15772.98352</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>94.95</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Apple iPhone XR - 128GB - Factory Unlocked - Very Good Condition</t>
+          <t>Samsung Galaxy S20 Ultra 5G SM-G988U - 128GB Cosmic Black (Unlocked) Smartphone</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>70412.2883958</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>264.95</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Magsafe Wireless Charger Magnetic Fast Charger For iPhone 15 14 13 12 11 Pro Max</t>
+          <t>Samsung Galaxy Note20 5G SM-N981U - 128GB -  (Unlocked)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2672.9573858</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>199</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 - 128GB - Factory Unlocked - Very Good Condition</t>
+          <t>Samsung Galaxy S10e/S10/S10+ Plus - Verizon/T-Mobile/AT&amp;T Or Unlocked- Excellent</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>92945.1219958</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>104.99</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Apple Watch Series 3 38mm 42mm GPS + WiFi + Bluetooth Gold Gray Silver - Good</t>
+          <t>Samsung Galaxy S20 / S20+ /S20 FE 5G - Unlocked/T-Mobile/Verizon/AT&amp;T- Excellent</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>23938.3190958</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>156.95</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Apple MacBook Pro Mneh3ll/a 2022 All Colors M2 - 8GB -10 GPU -  13.3" 256GB SSD</t>
+          <t>For Samsung Galaxy S22 S23 S21 Plus S22 Ultra Case Shockproof Heavy Duty Cover</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>253212.71758</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>7.59</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Apple Macbook Air 13 Laptop | i5 8GB + 512GB SSD | Ultra Light | MacOS+Warranty</t>
+          <t>Samsung Galaxy S20 5G G981U - 128GB - Gray (Unlocked) (MUST READ DESCRIPTION)</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>64500.23618</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>122.5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 - 64GB - Factory Unlocked - Pre-Owned Good Condition</t>
+          <t>Samsung Galaxy S20+ Plus 5G SM-G986U 128GB Unlocked Smartphone - Very Good</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>78862.10099579999</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>204.95</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Apple iPhone 14 Pro 128GB 256GB A2650 Factory Unlocked Smartphone Brand New</t>
+          <t>Samsung Galaxy S9 Unlocked | T-Mobile AT&amp;T Verizon | 64GB 4G Smartphone Good</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>260533.0718958</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>159</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 64GB Factory Unlocked AT&amp;T T-Mobile Verizon Fair Condition</t>
+          <t>Samsung Galaxy S10e G970U 128GB Factory Unlocked Android Smartphone -</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>82794.08045899999</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>154</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Apple iPad 6th 9.7" 2018 Wifi or Unlocked - 32GB 128GB - Gray Silver Gold </t>
+          <t>IN-BOX Samsung Galaxy S21+ Plus 5G SM-G996U 128GB Fully Unlocked EXCELLENT</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>39390.209737</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>319.95</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Apple iPhone 7 Plus - 128GB - All Colors - Unlocked - Good Condition</t>
+          <t>Samsung Galaxy A42 5G 128GB Unlocked Smartphone - Good</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>35489.21292</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>114.95</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Apple iPhone 6S (Excellent Condition) Factory Unlocked, Verizon, AT&amp;T, T-Mobile</t>
+          <t>Samsung Galaxy A14 4G LTE 128GB Dual SIM GSM Factory Unlocked Smartphone NEW</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>14083.021</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>139.95</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 Pro Max 128/256/512GB  Unlocked Very Good Condition</t>
+          <t>Samsung Galaxy A03s SM-A037U 32GB / 64GB Unlocked T-Mobile AT&amp;T Verizon</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>151814.96638</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>59.99</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Apple iphone 1st generation-iphone 3G-iphone 3GS Unlocked-Tested-Works well</t>
+          <t>Samsung Galaxy S7 SM-G930V - 32GB - Black Onyx (Carrier Unlocked)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>11514.2779696</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>19</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 Mini 128GB - T-Mobile / Metro - 5G Smartphone - Good Condition!</t>
+          <t>Samsung N960 Galaxy Note 9 128GB Unlocked 4G LTE Android Smartphone - Good</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>104211.5387958</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>154.95</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2021 Apple iPad 9th Gen 64/256GB WiFi 10.2"</t>
+          <t>New ListingSamsung Galaxy S8 64GB SM-G950U Midnight Black (T-Mobile) Smartphone</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>85621.9510758</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>64.95</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>99%N ew Apple iphone 4s 8-16-32-64GB Black/White UNlocked(GSM+CDMA) Grade A+</t>
+          <t>Samsung Galaxy Note 10 | Note 10+ Plus 256GB - (Unlocked) Verizon T-Mobile AT&amp;T</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>9291.9772558</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>219.95</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Apple Watch Series 3 38mm 42mm GPS + WiFi + Cellular Pink Gold Space Gray Silver</t>
+          <t>Samsung Galaxy S21+ Plus 128GB | 256GB 5G FACTORY UNLOCKED Smartphone -VERY GOOD</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>20276.7336358</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>258</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Apple iPhone X | XR | XS | XS Max - 64GB 128GB 256GB - Verizon GSM Unlocked AT&amp;T</t>
+          <t>Samsung Galaxy A10e SM-A102U - 32GB - Charcoal Black (T-Mobile) Great Condition</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>49276.49047899999</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>17.5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Apple iPhone 7+ Plus 32GB/128GB/256GB Verizon Unlocked T-Mobile AT&amp;T Smartphone</t>
+          <t>Samsung Galaxy G998U S21 Ultra 5G 128GB Unlocked Smartphone</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>33796.4337958</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>329.99</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Apple AirPods Pro (2nd Generation) Gen 2 - Excellent</t>
+          <t>Samsung Galaxy S22 Ultra SM-S908U - 256GB - Burgundy (Unlocked)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>45062.8505958</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>335</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 Pro 256GB Unlocked AT&amp;T T-Mobile Verizon Very Good Condition</t>
+          <t>Samsung Galaxy S21 | S21+ 5G 128GB 256GB - Unlocked Verizon T-Mobile AT&amp;T Metro</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>109833.480779</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>204.95</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 Pro Max 64/256/512GB AT&amp;T Sprint T-Mobile Unlocked Verizon Fair</t>
+          <t>Samsung Galaxy A14 5G (A146M) 128GB GSM Factory Unlocked Android (NEW)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>112661.3513958</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>182.95</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Apple iPhone 14 Pro Max 256GB ( Unlocked)  US E Sim - Excellent</t>
+          <t>Samsung Galaxy S10 | S10 Plus | S10e - 128GB | 512GB - (Unlocked) - Good</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>263349.6760958</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>129.95</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>APPLE MACBOOK PRO 15" | R9 GFX *HUGE 2TB SSD* 16GB | QUAD CORE i7 3.7Gh | RETINA</t>
+          <t>NEW UNLOCKED SAMSUNG GALAXY NOTE 20 5G SM-N981U 128GB ALL COLORS/MEMORY GSM+CDMA</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>164771.3457</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>305.69</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 512GB A2482 5G Factory Unlocked Brand New</t>
+          <t>Samsung Galaxy A54 5G 128GB SM-A546 50 MP (Unlocked T-Mobile AT&amp;T) Fedex 2 Day</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>185893.0605958</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>249.99</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Apple iphone 7/7 plus 32GB/128GB Unlocked Verizon tmobile at&amp;t Smartphone LTE</t>
+          <t>Samsung Galaxy S20 5G Unlocked G981U 128GB Android Smartphone Broken Parts</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>25067.77738</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>34</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 mini 128GB Factory Unlocked AT&amp;T T-Mobile Verizon Fair Condition</t>
+          <t>Samsung Galaxy S9 SM-G960U 64GB GSM Unlocked for AT&amp;T T-Mobile Verizon</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>74625.928279</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>119.99</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Lot of 5 Mix Apple iPods/iPhones for Scrap, Parts or Gold | iPhone 4 - iPhone XR</t>
+          <t>NEW Samsung Galaxy A50 SM-A505F - 128GB Black (DUAL SIM-UNLOCKED) Smartphone</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>9855.298095800001</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>140</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 64GB Factory Unlocked AT&amp;T T-Mobile Verizon Good Condition</t>
+          <t>Samsung Galaxy S10e SM-G970U Factory Unlocked 128GB Prism Black Good</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>90117.25137899999</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>109.99</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Apple Watch Series 5 40mm 44mm GPS+ WIFI + LTE UNLOCKED Gold Gray Silver - Good</t>
+          <t xml:space="preserve">Samsung Galaxy S20 5G Unlocked G981U 128GB Android Smartphone Excellent </t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>42246.2463958</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>208.99</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 - 128GB 256GB 512GB - All Colors - Excellent Condition</t>
+          <t>Unlocked Samsung Galaxy Folder G1600 Dual SIM LTE Flip SmartPhone- New Sealed</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>141675.19126</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>112</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 Pro Max 64GB Unlocked AT&amp;T T-Mobile Verizon Very Good Condition</t>
+          <t>NEW UNLOCKED SAMSUNG GALAXY S21 5G SM-G991U ALL COLORS AND MEMORY GSM+CDMA</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>112650.084979</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>312.78</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Apple iPhone 12 64GB Factory Unlocked AT&amp;T T-Mobile Verizon Very Good Condition</t>
+          <t>NEW in Box Samsung Galaxy S9+Plus SM-G965U 64GB Black GSM Unlocked ATT  T-Mobile</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>92933.855579</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>189.99</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Apple iPhone XR 64GB Factory Unlocked Smartphone - Very Good</t>
+          <t>Samsung G998 Galaxy S21 Ultra 5G 128GB Unlocked Smartphone - Very Good</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>61951.20937899999</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>354.95</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 mini 128GB Factory Unlocked AT&amp;T T-Mobile Verizon Very Good</t>
+          <t>Samsung Galaxy S21 5G G991U 128GB Fully Unlocked Smartphone - Good</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>125324.803879</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>209.99</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 Pro Max 256GB Unlocked AT&amp;T T-Mobile Verizon Very Good Condition</t>
+          <t>Samsung S20+ Plus 5G Unlocked G986U 128GB Android Smartphone Broken Parts</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>125324.803879</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>48</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 mini 128GB Factory Unlocked AT&amp;T T-Mobile Verizon Good Condition</t>
+          <t>Samsung Galaxy Note9 N960U - 128gb - Purple (Unlocked) (MUST READ DESCRIPTION)</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>116874.991279</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>76</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Apple airpods(3rd generation) Bluetooth wireless earphone charging case - white</t>
+          <t>NEW UNLOCKED SAMSUNG GALAXY S22 ULTRA 5G SM-S908U ALL COLORS AND MEMORY GSM+CDMA</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>13961.9070194</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>657.88</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Apple iPhone 12, 64/ 128GB -  Sprint Locked - Refurbished Grade A All colors</t>
+          <t>Samsung Galaxy S8 | S8+ Plus 64GB Unlocked Verizon T-Mobile AT&amp;T Metro Sprint</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>74637.1946958</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>94.95</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Apple iPhone 13 Pro 128GB Unlocked (GSM  and CDMA)  Excellent</t>
+          <t>Samsung Galaxy A32 5G - 64GB - (Unlocked) Verizon AT&amp;T T-Mobile Metro Cricket</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>187301.3626958</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>104.95</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Apple iPhone XR 64GB Factory Unlocked AT&amp;T T-Mobile Verizon Very Good Condition</t>
+          <t>Samsung Galaxy A01 SM-A015V - 16GB - Black (Verizon) (Single SIM)</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>57726.303079</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Apple iPhone XR - 64GB - Factory Unlocked - Good Condition</t>
+          <t>Samsung Galaxy Note 20 Ultra Unlocked N986U 128GB-Good</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>61680.8153758</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Monday, October 9, 2023--10:38:31 PM</t>
-        </is>
+        <v>349.99</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy S20 FE 5G - 128GB - Factory Unlocked - Excellent Condition</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>189.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>